<commit_message>
updated entries for load times
</commit_message>
<xml_diff>
--- a/index_build_times.xlsx
+++ b/index_build_times.xlsx
@@ -98,6 +98,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -119,12 +120,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -331,12 +334,12 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -528,7 +531,10 @@
         <f aca="false">(2.61356+2.62787+2.60664+2.66948+2.60817)/5</f>
         <v>2.625144</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="9" t="n">
+        <f aca="false">(203.385+203.583+204.463+204.39+203.633)/5</f>
+        <v>203.8908</v>
+      </c>
       <c r="E14" s="9" t="n">
         <f aca="false">(15.8809+15.8799+15.9602+16.2733+15.8961)/5</f>
         <v>15.97808</v>
@@ -546,7 +552,10 @@
         <f aca="false">(2.48563+2.26274+2.26329+2.28168+2.26243)/5</f>
         <v>2.311154</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9" t="n">
+        <f aca="false">(6.11628+6.10135+6.11597+6.1265+6.14355)/5</f>
+        <v>6.12073</v>
+      </c>
       <c r="E15" s="9" t="n">
         <f aca="false">(2.2143+2.28192+2.21146+2.21143+2.2129)/5</f>
         <v>2.226402</v>
@@ -564,7 +573,10 @@
         <f aca="false">(43.0941+39.6687+37.8384+38.0169+38.5331)/5</f>
         <v>39.43024</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="9" t="n">
+        <f aca="false">(488.498+482.918+485.014+484.759+481.954)/5</f>
+        <v>484.6286</v>
+      </c>
       <c r="E16" s="9" t="n">
         <f aca="false">(304.153+306.382+299.326+299.917+302.547)/5</f>
         <v>302.465</v>
@@ -582,7 +594,10 @@
         <f aca="false">(50.4878+50.0191+50.2795+50.4124+51.2379)/5</f>
         <v>50.48734</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="9" t="n">
+        <f aca="false">(2070.61+2136.17+2025.84+1536.91+1697.72)/5</f>
+        <v>1893.45</v>
+      </c>
       <c r="E17" s="9" t="n">
         <f aca="false">(260.704+258.935+260.797+259.026+258.224)/5</f>
         <v>259.5372</v>
@@ -600,7 +615,10 @@
         <f aca="false">(3.3197+3.62666+3.32007+3.31533+3.31798)/5</f>
         <v>3.379948</v>
       </c>
-      <c r="D18" s="9"/>
+      <c r="D18" s="9" t="n">
+        <f aca="false">(159.598+162.842+160.258+163.46+164.336)/5</f>
+        <v>162.0988</v>
+      </c>
       <c r="E18" s="9" t="n">
         <f aca="false">(3.2725+3.21404+3.5232+3.29191+3.39547)/5</f>
         <v>3.339424</v>
@@ -620,7 +638,7 @@
       </c>
       <c r="D19" s="9" t="n">
         <f aca="false">SUM(D14:D18)</f>
-        <v>0</v>
+        <v>2750.18893</v>
       </c>
       <c r="E19" s="9" t="n">
         <f aca="false">SUM(E14:E18)</f>

</xml_diff>

<commit_message>
finished averaging load times
</commit_message>
<xml_diff>
--- a/index_build_times.xlsx
+++ b/index_build_times.xlsx
@@ -200,7 +200,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,6 +258,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,7 +345,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -709,71 +713,176 @@
       <c r="A24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="12"/>
+      <c r="B24" s="15" t="n">
+        <f aca="false">(0.148542+0.148461+0.147445+0.148781+0.148514)/5</f>
+        <v>0.1483486</v>
+      </c>
+      <c r="C24" s="15" t="n">
+        <f aca="false">(0.22119+0.195683+0.196896+0.195851+0.200137)/5</f>
+        <v>0.2019514</v>
+      </c>
+      <c r="D24" s="15" t="n">
+        <f aca="false">(1.02987+1.04242+1.02666+1.0302+1.03145)/5</f>
+        <v>1.03212</v>
+      </c>
+      <c r="E24" s="15" t="n">
+        <f aca="false">(15.0838+15.8622+15.2584+15.4685+15.2169)/5</f>
+        <v>15.37796</v>
+      </c>
+      <c r="F24" s="15" t="n">
+        <f aca="false">(1.07828+1.05154+1.03035+1.03241+1.02617)/5</f>
+        <v>1.04375</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="12"/>
+      <c r="B25" s="15" t="n">
+        <f aca="false">(0.656544+0.656577+0.656983+0.657071+0.657465)/5</f>
+        <v>0.656928</v>
+      </c>
+      <c r="C25" s="15" t="n">
+        <f aca="false">(0.762904+0.762778+0.763616+0.763524+0.764375)/5</f>
+        <v>0.7634394</v>
+      </c>
+      <c r="D25" s="15" t="n">
+        <f aca="false">(3.61774+3.61151+3.61306+3.65721+3.64153)/5</f>
+        <v>3.62821</v>
+      </c>
+      <c r="E25" s="15" t="n">
+        <f aca="false">(218.66+218.778+221.719+221.025+218.572)/5</f>
+        <v>219.7508</v>
+      </c>
+      <c r="F25" s="15" t="n">
+        <f aca="false">(3.62415+3.61532+3.61154+3.6341+3.61377)/5</f>
+        <v>3.619776</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="15" t="n">
+        <f aca="false">(3.07683+3.06376+3.13867+3.07326+3.06826)/5</f>
+        <v>3.084156</v>
+      </c>
+      <c r="C26" s="15" t="n">
+        <f aca="false">(3.84828+3.85047+3.85387+3.85881+3.85288)/5</f>
+        <v>3.852862</v>
+      </c>
+      <c r="D26" s="15" t="n">
+        <f aca="false">(22.8852+22.8723+23.049+24.2356+22.8745)/5</f>
+        <v>23.18332</v>
+      </c>
+      <c r="E26" s="15" t="n">
+        <f aca="false">(700.848+694.558+690.941+714.705+693.824)/5</f>
+        <v>698.9752</v>
+      </c>
+      <c r="F26" s="15" t="n">
+        <f aca="false">(23.0711+22.9609+22.9109+24.6303+22.8736)/5</f>
+        <v>23.28936</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="12"/>
+      <c r="B27" s="15" t="n">
+        <f aca="false">(11.3389+11.4321+11.58+11.3597+11.3709)/5</f>
+        <v>11.41632</v>
+      </c>
+      <c r="C27" s="15" t="n">
+        <f aca="false">(13.3618+13.2946+13.3055+13.3022+13.301)/5</f>
+        <v>13.31302</v>
+      </c>
+      <c r="D27" s="15" t="n">
+        <f aca="false">(53.0528+53.2677+53.8663+53.3803+53.6128)/5</f>
+        <v>53.43598</v>
+      </c>
+      <c r="E27" s="15" t="n">
+        <f aca="false">(3231.63+3276.54+3198.06+3075.7+2998.18)/5</f>
+        <v>3156.022</v>
+      </c>
+      <c r="F27" s="15" t="n">
+        <f aca="false">(662.312+397.023+349.231+398.163+349.231+371.301)/5</f>
+        <v>505.4522</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="12"/>
+      <c r="B28" s="15" t="n">
+        <f aca="false">(2.25127+2.25606+2.4884+2.25569+2.25729)/5</f>
+        <v>2.301742</v>
+      </c>
+      <c r="C28" s="15" t="n">
+        <f aca="false">(2.90764+2.90838+2.90881+2.90827+2.91081)/5</f>
+        <v>2.908782</v>
+      </c>
+      <c r="D28" s="15" t="n">
+        <f aca="false">(18.2144+18.2161+18.7175+18.3709+18.2204)/5</f>
+        <v>18.34786</v>
+      </c>
+      <c r="E28" s="15" t="n">
+        <f aca="false">(36.996+39.076+36.1302+34.3196+37.0837)/5</f>
+        <v>36.7211</v>
+      </c>
+      <c r="F28" s="15" t="n">
+        <f aca="false">(20.5763+20.6189+20.6514+20.8378+20.6164)/5</f>
+        <v>20.66016</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="12"/>
+      <c r="B29" s="15" t="n">
+        <f aca="false">(0.16176+0.161215+0.162113+0.16176+0.16247)/5</f>
+        <v>0.1618636</v>
+      </c>
+      <c r="C29" s="15" t="n">
+        <f aca="false">(0.214602+0.214146+0.214403+0.214654+0.214532)/5</f>
+        <v>0.2144674</v>
+      </c>
+      <c r="D29" s="15" t="n">
+        <f aca="false">(1.145+1.15569+1.14106+1.14331+1.14345)/5</f>
+        <v>1.145702</v>
+      </c>
+      <c r="E29" s="15" t="n">
+        <f aca="false">(13.1867+13.345+13.3665+13.1004+13.1382)/5</f>
+        <v>13.22736</v>
+      </c>
+      <c r="F29" s="15" t="n">
+        <f aca="false">(1.14281+1.14335+1.14226+1.14081+1.14028)/5</f>
+        <v>1.141902</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="12"/>
+      <c r="B30" s="15" t="n">
+        <f aca="false">SUM(B24:B29)</f>
+        <v>17.7693582</v>
+      </c>
+      <c r="C30" s="15" t="n">
+        <f aca="false">SUM(C24:C29)</f>
+        <v>21.2545222</v>
+      </c>
+      <c r="D30" s="15" t="n">
+        <f aca="false">SUM(D24:D29)</f>
+        <v>100.773192</v>
+      </c>
+      <c r="E30" s="15" t="n">
+        <f aca="false">SUM(E24:E29)</f>
+        <v>4140.07442</v>
+      </c>
+      <c r="F30" s="15" t="n">
+        <f aca="false">SUM(F24:F29)</f>
+        <v>555.207148</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>